<commit_message>
Started Latex Beamer Template
still sooo slow.
</commit_message>
<xml_diff>
--- a/Logistics/LectureSchedule/Lecture_Schedule_SS2022.xlsx
+++ b/Logistics/LectureSchedule/Lecture_Schedule_SS2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdrews/Nextcloud/esd_teach/geophyscis_BSc_SoSe22/Logistics/LectureSchedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F9CE70-9D13-D649-AAC2-B448F2A6DEBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E5307F-7270-C644-9805-C956F9A8A809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1683,8 +1683,8 @@
   </sheetPr>
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1855,7 +1855,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="21">
-        <v>44307</v>
+        <v>44672</v>
       </c>
       <c r="F15" s="27" t="s">
         <v>65</v>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="E17" s="24">
         <f>E15+7</f>
-        <v>44314</v>
+        <v>44679</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>61</v>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="E19" s="24">
         <f t="shared" si="0"/>
-        <v>44321</v>
+        <v>44686</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>43</v>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="E21" s="24">
         <f t="shared" si="0"/>
-        <v>44328</v>
+        <v>44693</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>45</v>
@@ -2032,7 +2032,7 @@
       </c>
       <c r="E23" s="24">
         <f t="shared" si="0"/>
-        <v>44335</v>
+        <v>44700</v>
       </c>
       <c r="F23" s="26" t="s">
         <v>46</v>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="E25" s="22">
         <f t="shared" si="0"/>
-        <v>44342</v>
+        <v>44707</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>14</v>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="E27" s="24">
         <f t="shared" si="0"/>
-        <v>44349</v>
+        <v>44714</v>
       </c>
       <c r="F27" s="26" t="s">
         <v>49</v>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="E29" s="22">
         <f t="shared" si="0"/>
-        <v>44356</v>
+        <v>44721</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="6" t="s">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="E31" s="22">
         <f t="shared" si="0"/>
-        <v>44363</v>
+        <v>44728</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>5</v>
@@ -2256,7 +2256,7 @@
       </c>
       <c r="E33" s="24">
         <f t="shared" si="0"/>
-        <v>44370</v>
+        <v>44735</v>
       </c>
       <c r="F33" s="28" t="s">
         <v>53</v>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="E35" s="24">
         <f t="shared" si="0"/>
-        <v>44377</v>
+        <v>44742</v>
       </c>
       <c r="F35" s="27" t="s">
         <v>51</v>
@@ -2345,7 +2345,7 @@
       </c>
       <c r="E37" s="24">
         <f t="shared" si="0"/>
-        <v>44384</v>
+        <v>44749</v>
       </c>
       <c r="F37" s="26" t="s">
         <v>54</v>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="E39" s="24">
         <f t="shared" si="0"/>
-        <v>44391</v>
+        <v>44756</v>
       </c>
       <c r="F39" s="26" t="s">
         <v>56</v>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="E41" s="24">
         <f t="shared" si="0"/>
-        <v>44398</v>
+        <v>44763</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>59</v>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="E43" s="24">
         <f t="shared" si="0"/>
-        <v>44405</v>
+        <v>44770</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>58</v>
@@ -2498,8 +2498,7 @@
         <v>67</v>
       </c>
       <c r="E44" s="39">
-        <f t="shared" si="0"/>
-        <v>44775</v>
+        <v>44774</v>
       </c>
       <c r="F44" s="40" t="s">
         <v>68</v>

</xml_diff>